<commit_message>
Adding the code for Phase 2 modified
</commit_message>
<xml_diff>
--- a/project/phase2_results.xlsx
+++ b/project/phase2_results.xlsx
@@ -486,19 +486,19 @@
         <v>3.158293710110962</v>
       </c>
       <c r="D2" t="n">
-        <v>6.114621593431533</v>
+        <v>6.109631711691939</v>
       </c>
       <c r="E2" t="n">
-        <v>3.18393426821774</v>
+        <v>3.180114391530244</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01892809485989844</v>
+        <v>0.01393821312030408</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02564055810677779</v>
+        <v>0.02182068141928184</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03187022113278102</v>
+        <v>0.02589239121033066</v>
       </c>
     </row>
     <row r="3">
@@ -512,19 +512,19 @@
         <v>1.132221084228233</v>
       </c>
       <c r="D3" t="n">
-        <v>1.327006606049438</v>
+        <v>1.32443318853413</v>
       </c>
       <c r="E3" t="n">
-        <v>1.125112170545788</v>
+        <v>1.128411107423878</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0007815854401191924</v>
+        <v>-0.003355002955427233</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.00710891368244515</v>
+        <v>-0.003809976804354465</v>
       </c>
       <c r="H3" t="n">
-        <v>0.007151750103622342</v>
+        <v>0.005076609900380817</v>
       </c>
     </row>
     <row r="4">
@@ -538,19 +538,19 @@
         <v>8.302044618221775</v>
       </c>
       <c r="D4" t="n">
-        <v>7.504739969499223</v>
+        <v>7.502994929472846</v>
       </c>
       <c r="E4" t="n">
-        <v>8.299169124719748</v>
+        <v>8.301364246861349</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.001421944102956374</v>
+        <v>-0.003166984129333805</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.002875493502026316</v>
+        <v>-0.0006803713604259798</v>
       </c>
       <c r="H4" t="n">
-        <v>0.003207863449732232</v>
+        <v>0.003239242760822365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>